<commit_message>
edits for main site
</commit_message>
<xml_diff>
--- a/database/capsules_spreadsheets/Fall 2021 Capsules.xlsx
+++ b/database/capsules_spreadsheets/Fall 2021 Capsules.xlsx
@@ -8,9 +8,9 @@
   </sheets>
   <definedNames>
     <definedName localSheetId="1" name="LOCKED_CAPSULES">'Series Info'!$A$1:$R$22</definedName>
-    <definedName name="Examples">'Fall 2021'!$A$3:$Y$3</definedName>
+    <definedName name="Examples">'Fall 2021'!$A$3:$Z$3</definedName>
     <definedName localSheetId="1" name="Examples">#REF!</definedName>
-    <definedName name="LOCKED_CAPSULES">'Fall 2021'!$A$1:$Y$88</definedName>
+    <definedName name="LOCKED_CAPSULES">'Fall 2021'!$A$1:$Z$88</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="225">
   <si>
     <t>title</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>showtime3</t>
+  </si>
+  <si>
+    <t>ticketing url</t>
   </si>
   <si>
     <t>public notes</t>
@@ -1510,15 +1513,15 @@
     <col customWidth="1" min="13" max="13" width="12.75"/>
     <col customWidth="1" min="14" max="14" width="9.0"/>
     <col customWidth="1" min="15" max="15" width="7.5"/>
-    <col customWidth="1" min="17" max="17" width="28.25"/>
-    <col customWidth="1" min="18" max="18" width="13.88"/>
-    <col customWidth="1" min="19" max="20" width="16.88"/>
-    <col customWidth="1" min="21" max="21" width="9.25"/>
-    <col customWidth="1" min="22" max="22" width="12.38"/>
-    <col customWidth="1" min="23" max="23" width="14.38"/>
-    <col customWidth="1" min="24" max="24" width="9.0"/>
-    <col customWidth="1" min="25" max="25" width="8.25"/>
-    <col customWidth="1" min="26" max="28" width="15.13"/>
+    <col customWidth="1" min="18" max="18" width="28.25"/>
+    <col customWidth="1" min="19" max="19" width="13.88"/>
+    <col customWidth="1" min="20" max="21" width="16.88"/>
+    <col customWidth="1" min="22" max="22" width="9.25"/>
+    <col customWidth="1" min="23" max="23" width="12.38"/>
+    <col customWidth="1" min="24" max="24" width="14.38"/>
+    <col customWidth="1" min="25" max="25" width="9.0"/>
+    <col customWidth="1" min="26" max="26" width="8.25"/>
+    <col customWidth="1" min="27" max="29" width="15.13"/>
   </cols>
   <sheetData>
     <row r="1" ht="33.75" customHeight="1">
@@ -1576,48 +1579,51 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4"/>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="T1" s="4"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="5"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
-      <c r="AB1" s="5"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="5"/>
     </row>
     <row r="2" ht="65.25" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="7">
         <f t="shared" ref="B2:B23" si="1">len(H2)</f>
         <v>495</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="12">
         <v>1990.0</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="12">
         <v>98.0</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" s="15">
         <v>42457.0</v>
@@ -1629,50 +1635,51 @@
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="20"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="19"/>
       <c r="T2" s="20"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="7"/>
       <c r="W2" s="20"/>
       <c r="X2" s="20"/>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
       <c r="AA2" s="20"/>
-      <c r="AB2" s="7"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="7"/>
     </row>
     <row r="3" ht="101.25" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="7">
         <f t="shared" si="1"/>
         <v>477</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="22">
         <v>1934.0</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" s="24">
         <v>76.0</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K3" s="15">
         <v>42458.0</v>
@@ -1684,50 +1691,51 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="19"/>
+      <c r="Q3" s="17"/>
       <c r="R3" s="19"/>
-      <c r="S3" s="20"/>
+      <c r="S3" s="19"/>
       <c r="T3" s="20"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="7"/>
       <c r="W3" s="20"/>
       <c r="X3" s="20"/>
       <c r="Y3" s="20"/>
       <c r="Z3" s="20"/>
       <c r="AA3" s="20"/>
-      <c r="AB3" s="7"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="7">
         <f t="shared" si="1"/>
         <v>453</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G4" s="28">
         <v>1994.0</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" s="30">
         <v>44469.0</v>
@@ -1739,51 +1747,52 @@
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="32"/>
-      <c r="R4" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S4" s="33"/>
+      <c r="Q4" s="32"/>
+      <c r="S4" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T4" s="33"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="34"/>
       <c r="W4" s="33"/>
       <c r="X4" s="33"/>
       <c r="Y4" s="33"/>
       <c r="Z4" s="33"/>
       <c r="AA4" s="33"/>
-      <c r="AB4" s="34"/>
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="34"/>
     </row>
     <row r="5">
       <c r="A5" s="25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7">
         <f t="shared" si="1"/>
         <v>450</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G5" s="28">
         <v>2001.0</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K5" s="30">
         <v>44469.0</v>
@@ -1795,51 +1804,52 @@
       <c r="N5" s="32"/>
       <c r="O5" s="32"/>
       <c r="P5" s="32"/>
-      <c r="R5" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="S5" s="33"/>
+      <c r="Q5" s="32"/>
+      <c r="S5" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="T5" s="33"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="33"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="34"/>
       <c r="W5" s="33"/>
       <c r="X5" s="33"/>
       <c r="Y5" s="33"/>
       <c r="Z5" s="33"/>
       <c r="AA5" s="33"/>
-      <c r="AB5" s="34"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="34"/>
     </row>
     <row r="6">
       <c r="A6" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" s="7">
         <f t="shared" si="1"/>
         <v>440</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G6" s="28">
         <v>2020.0</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K6" s="30">
         <v>44470.0</v>
@@ -1855,51 +1865,52 @@
       </c>
       <c r="O6" s="32"/>
       <c r="P6" s="32"/>
-      <c r="R6" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="S6" s="33"/>
+      <c r="Q6" s="32"/>
+      <c r="S6" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="T6" s="33"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="34"/>
       <c r="W6" s="33"/>
       <c r="X6" s="33"/>
       <c r="Y6" s="33"/>
       <c r="Z6" s="33"/>
       <c r="AA6" s="33"/>
-      <c r="AB6" s="34"/>
+      <c r="AB6" s="33"/>
+      <c r="AC6" s="34"/>
     </row>
     <row r="7">
       <c r="A7" s="25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7">
         <f t="shared" si="1"/>
         <v>448</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G7" s="28">
         <v>1987.0</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K7" s="30">
         <v>44471.0</v>
@@ -1911,51 +1922,52 @@
       <c r="N7" s="32"/>
       <c r="O7" s="32"/>
       <c r="P7" s="32"/>
-      <c r="R7" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S7" s="33"/>
+      <c r="Q7" s="32"/>
+      <c r="S7" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="T7" s="33"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="34"/>
       <c r="W7" s="33"/>
       <c r="X7" s="33"/>
       <c r="Y7" s="33"/>
       <c r="Z7" s="33"/>
       <c r="AA7" s="33"/>
-      <c r="AB7" s="34"/>
+      <c r="AB7" s="33"/>
+      <c r="AC7" s="34"/>
     </row>
     <row r="8">
       <c r="A8" s="25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B8" s="7">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G8" s="28">
         <v>1989.0</v>
       </c>
       <c r="H8" s="41" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K8" s="30">
         <v>44471.0</v>
@@ -1971,54 +1983,55 @@
       </c>
       <c r="O8" s="32"/>
       <c r="P8" s="32"/>
-      <c r="Q8" s="27" t="s">
-        <v>64</v>
-      </c>
+      <c r="Q8" s="32"/>
       <c r="R8" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="S8" s="33"/>
+      <c r="S8" s="27" t="s">
+        <v>66</v>
+      </c>
       <c r="T8" s="33"/>
-      <c r="U8" s="34"/>
-      <c r="V8" s="33"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="34"/>
       <c r="W8" s="33"/>
       <c r="X8" s="33"/>
       <c r="Y8" s="33"/>
       <c r="Z8" s="33"/>
       <c r="AA8" s="33"/>
-      <c r="AB8" s="34"/>
+      <c r="AB8" s="33"/>
+      <c r="AC8" s="34"/>
     </row>
     <row r="9">
       <c r="A9" s="25" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" s="7">
         <f t="shared" si="1"/>
         <v>450</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G9" s="28">
         <v>2001.0</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K9" s="45">
         <v>44476.0</v>
@@ -2030,51 +2043,52 @@
       <c r="N9" s="39"/>
       <c r="O9" s="46"/>
       <c r="P9" s="37"/>
-      <c r="R9" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S9" s="33"/>
+      <c r="Q9" s="37"/>
+      <c r="S9" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T9" s="33"/>
-      <c r="U9" s="34"/>
-      <c r="V9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="34"/>
       <c r="W9" s="33"/>
       <c r="X9" s="33"/>
       <c r="Y9" s="33"/>
       <c r="Z9" s="33"/>
       <c r="AA9" s="33"/>
-      <c r="AB9" s="34"/>
+      <c r="AB9" s="33"/>
+      <c r="AC9" s="34"/>
     </row>
     <row r="10">
       <c r="A10" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" s="7">
         <f t="shared" si="1"/>
         <v>446</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G10" s="28">
         <v>1996.0</v>
       </c>
       <c r="H10" s="47" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K10" s="48">
         <v>44476.0</v>
@@ -2086,52 +2100,53 @@
       <c r="N10" s="39"/>
       <c r="O10" s="46"/>
       <c r="P10" s="37"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="S10" s="33"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="T10" s="33"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="33"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="34"/>
       <c r="W10" s="33"/>
       <c r="X10" s="33"/>
       <c r="Y10" s="33"/>
       <c r="Z10" s="33"/>
       <c r="AA10" s="33"/>
-      <c r="AB10" s="34"/>
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="34"/>
     </row>
     <row r="11">
       <c r="A11" s="25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B11" s="7">
         <f t="shared" si="1"/>
         <v>459</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G11" s="28">
         <v>2021.0</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K11" s="48">
         <v>44477.0</v>
@@ -2147,52 +2162,53 @@
       </c>
       <c r="O11" s="32"/>
       <c r="P11" s="32"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="S11" s="33"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="T11" s="33"/>
-      <c r="U11" s="34"/>
-      <c r="V11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="34"/>
       <c r="W11" s="33"/>
       <c r="X11" s="33"/>
       <c r="Y11" s="33"/>
       <c r="Z11" s="33"/>
       <c r="AA11" s="33"/>
-      <c r="AB11" s="34"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="34"/>
     </row>
     <row r="12">
       <c r="A12" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B12" s="7">
         <f t="shared" si="1"/>
         <v>455</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G12" s="28">
         <v>1973.0</v>
       </c>
       <c r="H12" s="51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K12" s="48">
         <v>44478.0</v>
@@ -2204,51 +2220,52 @@
       <c r="N12" s="32"/>
       <c r="O12" s="32"/>
       <c r="P12" s="32"/>
-      <c r="R12" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S12" s="33"/>
+      <c r="Q12" s="32"/>
+      <c r="S12" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="T12" s="33"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="33"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="34"/>
       <c r="W12" s="33"/>
       <c r="X12" s="33"/>
       <c r="Y12" s="33"/>
       <c r="Z12" s="33"/>
       <c r="AA12" s="33"/>
-      <c r="AB12" s="34"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="34"/>
     </row>
     <row r="13">
       <c r="A13" s="25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B13" s="7">
         <f t="shared" si="1"/>
         <v>445</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G13" s="28">
         <v>2006.0</v>
       </c>
       <c r="H13" s="51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K13" s="48">
         <v>44483.0</v>
@@ -2260,51 +2277,52 @@
       <c r="N13" s="32"/>
       <c r="O13" s="32"/>
       <c r="P13" s="32"/>
-      <c r="R13" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S13" s="33"/>
+      <c r="Q13" s="32"/>
+      <c r="S13" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T13" s="33"/>
-      <c r="U13" s="34"/>
-      <c r="V13" s="33"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="34"/>
       <c r="W13" s="33"/>
       <c r="X13" s="33"/>
       <c r="Y13" s="33"/>
       <c r="Z13" s="33"/>
       <c r="AA13" s="33"/>
-      <c r="AB13" s="34"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="34"/>
     </row>
     <row r="14">
       <c r="A14" s="25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B14" s="7">
         <f t="shared" si="1"/>
         <v>459</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G14" s="28">
         <v>1950.0</v>
       </c>
       <c r="H14" s="52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K14" s="48">
         <v>44483.0</v>
@@ -2316,51 +2334,52 @@
       <c r="N14" s="32"/>
       <c r="O14" s="32"/>
       <c r="P14" s="32"/>
-      <c r="R14" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="S14" s="33"/>
+      <c r="Q14" s="32"/>
+      <c r="S14" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="T14" s="33"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="33"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="34"/>
       <c r="W14" s="33"/>
       <c r="X14" s="33"/>
       <c r="Y14" s="33"/>
       <c r="Z14" s="33"/>
       <c r="AA14" s="33"/>
-      <c r="AB14" s="34"/>
+      <c r="AB14" s="33"/>
+      <c r="AC14" s="34"/>
     </row>
     <row r="15">
       <c r="A15" s="53" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B15" s="7">
         <f t="shared" si="1"/>
         <v>452</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G15" s="28">
         <v>2021.0</v>
       </c>
       <c r="H15" s="51" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I15" s="28" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K15" s="48">
         <v>44484.0</v>
@@ -2376,52 +2395,53 @@
       </c>
       <c r="O15" s="32"/>
       <c r="P15" s="32"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="S15" s="33"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="T15" s="33"/>
-      <c r="U15" s="34"/>
-      <c r="V15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="34"/>
       <c r="W15" s="33"/>
       <c r="X15" s="33"/>
       <c r="Y15" s="33"/>
       <c r="Z15" s="33"/>
       <c r="AA15" s="33"/>
-      <c r="AB15" s="34"/>
+      <c r="AB15" s="33"/>
+      <c r="AC15" s="34"/>
     </row>
     <row r="16">
       <c r="A16" s="25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B16" s="7">
         <f t="shared" si="1"/>
         <v>455</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F16" s="54" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G16" s="55">
         <v>1971.0</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K16" s="48">
         <v>44485.0</v>
@@ -2433,51 +2453,52 @@
       <c r="N16" s="56"/>
       <c r="O16" s="32"/>
       <c r="P16" s="32"/>
-      <c r="R16" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S16" s="33"/>
+      <c r="Q16" s="32"/>
+      <c r="S16" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="T16" s="33"/>
-      <c r="U16" s="34"/>
-      <c r="V16" s="33"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="34"/>
       <c r="W16" s="33"/>
       <c r="X16" s="33"/>
       <c r="Y16" s="33"/>
       <c r="Z16" s="33"/>
       <c r="AA16" s="33"/>
-      <c r="AB16" s="34"/>
+      <c r="AB16" s="33"/>
+      <c r="AC16" s="34"/>
     </row>
     <row r="17">
       <c r="A17" s="25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B17" s="7">
         <f t="shared" si="1"/>
         <v>452</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G17" s="28">
         <v>1950.0</v>
       </c>
       <c r="H17" s="51" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I17" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K17" s="48">
         <v>44490.0</v>
@@ -2489,52 +2510,53 @@
       <c r="N17" s="56"/>
       <c r="O17" s="32"/>
       <c r="P17" s="32"/>
-      <c r="Q17" s="57"/>
-      <c r="R17" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S17" s="33"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="57"/>
+      <c r="S17" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T17" s="33"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="33"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="34"/>
       <c r="W17" s="33"/>
       <c r="X17" s="33"/>
       <c r="Y17" s="33"/>
       <c r="Z17" s="33"/>
       <c r="AA17" s="33"/>
-      <c r="AB17" s="34"/>
+      <c r="AB17" s="33"/>
+      <c r="AC17" s="34"/>
     </row>
     <row r="18">
       <c r="A18" s="25" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B18" s="7">
         <f t="shared" si="1"/>
         <v>457</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G18" s="28">
         <v>1955.0</v>
       </c>
       <c r="H18" s="47" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K18" s="48">
         <v>44490.0</v>
@@ -2546,51 +2568,52 @@
       <c r="N18" s="58"/>
       <c r="O18" s="43"/>
       <c r="P18" s="37"/>
-      <c r="R18" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="S18" s="33"/>
+      <c r="Q18" s="37"/>
+      <c r="S18" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="T18" s="33"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="34"/>
       <c r="W18" s="33"/>
       <c r="X18" s="33"/>
       <c r="Y18" s="33"/>
       <c r="Z18" s="33"/>
       <c r="AA18" s="33"/>
-      <c r="AB18" s="34"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="34"/>
     </row>
     <row r="19">
       <c r="A19" s="25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B19" s="7">
         <f t="shared" si="1"/>
         <v>453</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G19" s="28">
         <v>2020.0</v>
       </c>
       <c r="H19" s="51" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I19" s="28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K19" s="48">
         <v>44491.0</v>
@@ -2606,51 +2629,52 @@
       </c>
       <c r="O19" s="43"/>
       <c r="P19" s="37"/>
-      <c r="R19" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="S19" s="33"/>
+      <c r="Q19" s="37"/>
+      <c r="S19" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="T19" s="33"/>
-      <c r="U19" s="34"/>
-      <c r="V19" s="33"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="34"/>
       <c r="W19" s="33"/>
       <c r="X19" s="33"/>
       <c r="Y19" s="33"/>
       <c r="Z19" s="33"/>
       <c r="AA19" s="33"/>
-      <c r="AB19" s="34"/>
+      <c r="AB19" s="33"/>
+      <c r="AC19" s="34"/>
     </row>
     <row r="20">
       <c r="A20" s="25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B20" s="7">
         <f t="shared" si="1"/>
         <v>457</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G20" s="28">
         <v>1939.0</v>
       </c>
       <c r="H20" s="35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K20" s="48">
         <v>44492.0</v>
@@ -2662,52 +2686,53 @@
       <c r="N20" s="32"/>
       <c r="O20" s="60"/>
       <c r="P20" s="32"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S20" s="33"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="T20" s="33"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="34"/>
       <c r="W20" s="33"/>
       <c r="X20" s="33"/>
       <c r="Y20" s="33"/>
       <c r="Z20" s="33"/>
       <c r="AA20" s="33"/>
-      <c r="AB20" s="34"/>
+      <c r="AB20" s="33"/>
+      <c r="AC20" s="34"/>
     </row>
     <row r="21">
       <c r="A21" s="25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B21" s="7">
         <f t="shared" si="1"/>
         <v>455</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G21" s="28">
         <v>1980.0</v>
       </c>
       <c r="H21" s="51" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K21" s="48">
         <v>44497.0</v>
@@ -2719,51 +2744,52 @@
       <c r="N21" s="32"/>
       <c r="O21" s="32"/>
       <c r="P21" s="32"/>
-      <c r="R21" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S21" s="33"/>
+      <c r="Q21" s="32"/>
+      <c r="S21" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T21" s="33"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="33"/>
+      <c r="U21" s="33"/>
+      <c r="V21" s="34"/>
       <c r="W21" s="33"/>
       <c r="X21" s="33"/>
       <c r="Y21" s="33"/>
       <c r="Z21" s="33"/>
       <c r="AA21" s="33"/>
-      <c r="AB21" s="34"/>
+      <c r="AB21" s="33"/>
+      <c r="AC21" s="34"/>
     </row>
     <row r="22">
       <c r="A22" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B22" s="7">
         <f t="shared" si="1"/>
         <v>453</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D22" s="50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G22" s="28">
         <v>1986.0</v>
       </c>
       <c r="H22" s="61" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K22" s="48">
         <v>44497.0</v>
@@ -2775,51 +2801,52 @@
       <c r="N22" s="32"/>
       <c r="O22" s="32"/>
       <c r="P22" s="32"/>
-      <c r="R22" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S22" s="33"/>
+      <c r="Q22" s="32"/>
+      <c r="S22" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T22" s="33"/>
-      <c r="U22" s="34"/>
-      <c r="V22" s="33"/>
+      <c r="U22" s="33"/>
+      <c r="V22" s="34"/>
       <c r="W22" s="33"/>
       <c r="X22" s="33"/>
       <c r="Y22" s="33"/>
       <c r="Z22" s="33"/>
       <c r="AA22" s="33"/>
-      <c r="AB22" s="34"/>
+      <c r="AB22" s="33"/>
+      <c r="AC22" s="34"/>
     </row>
     <row r="23">
       <c r="A23" s="25" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B23" s="7">
         <f t="shared" si="1"/>
         <v>441</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G23" s="28">
         <v>2021.0</v>
       </c>
       <c r="H23" s="51" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I23" s="28" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K23" s="48">
         <v>44498.0</v>
@@ -2835,42 +2862,43 @@
       </c>
       <c r="O23" s="32"/>
       <c r="P23" s="32"/>
-      <c r="R23" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="S23" s="33"/>
+      <c r="Q23" s="32"/>
+      <c r="S23" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="T23" s="33"/>
-      <c r="U23" s="34"/>
-      <c r="V23" s="33"/>
+      <c r="U23" s="33"/>
+      <c r="V23" s="34"/>
       <c r="W23" s="33"/>
       <c r="X23" s="33"/>
       <c r="Y23" s="33"/>
       <c r="Z23" s="33"/>
       <c r="AA23" s="33"/>
-      <c r="AB23" s="34"/>
+      <c r="AB23" s="33"/>
+      <c r="AC23" s="34"/>
     </row>
     <row r="24">
       <c r="A24" s="25" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="26"/>
       <c r="D24" s="25"/>
       <c r="E24" s="27"/>
       <c r="F24" s="25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G24" s="28">
         <v>2019.0</v>
       </c>
       <c r="H24" s="62" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I24" s="28" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K24" s="48">
         <v>44499.0</v>
@@ -2882,54 +2910,55 @@
       <c r="N24" s="32"/>
       <c r="O24" s="32"/>
       <c r="P24" s="32"/>
-      <c r="Q24" s="27" t="s">
-        <v>134</v>
-      </c>
+      <c r="Q24" s="32"/>
       <c r="R24" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="S24" s="33"/>
+        <v>135</v>
+      </c>
+      <c r="S24" s="27" t="s">
+        <v>66</v>
+      </c>
       <c r="T24" s="33"/>
-      <c r="U24" s="34"/>
-      <c r="V24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="34"/>
       <c r="W24" s="33"/>
       <c r="X24" s="33"/>
       <c r="Y24" s="33"/>
       <c r="Z24" s="33"/>
       <c r="AA24" s="33"/>
-      <c r="AB24" s="34"/>
+      <c r="AB24" s="33"/>
+      <c r="AC24" s="34"/>
     </row>
     <row r="25">
       <c r="A25" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B25" s="7">
         <f t="shared" ref="B25:B43" si="2">len(H25)</f>
         <v>457</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G25" s="28">
         <v>1945.0</v>
       </c>
       <c r="H25" s="62" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I25" s="28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K25" s="48">
         <v>44499.0</v>
@@ -2941,51 +2970,52 @@
       <c r="N25" s="32"/>
       <c r="O25" s="32"/>
       <c r="P25" s="32"/>
-      <c r="R25" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="S25" s="33"/>
+      <c r="Q25" s="32"/>
+      <c r="S25" s="27" t="s">
+        <v>66</v>
+      </c>
       <c r="T25" s="33"/>
-      <c r="U25" s="34"/>
-      <c r="V25" s="33"/>
+      <c r="U25" s="33"/>
+      <c r="V25" s="34"/>
       <c r="W25" s="33"/>
       <c r="X25" s="33"/>
       <c r="Y25" s="33"/>
       <c r="Z25" s="33"/>
       <c r="AA25" s="33"/>
-      <c r="AB25" s="34"/>
+      <c r="AB25" s="33"/>
+      <c r="AC25" s="34"/>
     </row>
     <row r="26">
       <c r="A26" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B26" s="7">
         <f t="shared" si="2"/>
         <v>459</v>
       </c>
       <c r="C26" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="25" t="s">
-        <v>31</v>
-      </c>
       <c r="E26" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G26" s="28">
         <v>1963.0</v>
       </c>
       <c r="H26" s="61" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K26" s="63">
         <v>44499.0</v>
@@ -2997,51 +3027,52 @@
       <c r="N26" s="32"/>
       <c r="O26" s="32"/>
       <c r="P26" s="32"/>
-      <c r="R26" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="S26" s="33"/>
+      <c r="Q26" s="32"/>
+      <c r="S26" s="27" t="s">
+        <v>66</v>
+      </c>
       <c r="T26" s="33"/>
-      <c r="U26" s="34"/>
-      <c r="V26" s="33"/>
+      <c r="U26" s="33"/>
+      <c r="V26" s="34"/>
       <c r="W26" s="33"/>
       <c r="X26" s="33"/>
       <c r="Y26" s="33"/>
       <c r="Z26" s="33"/>
       <c r="AA26" s="33"/>
-      <c r="AB26" s="34"/>
+      <c r="AB26" s="33"/>
+      <c r="AC26" s="34"/>
     </row>
     <row r="27">
       <c r="A27" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B27" s="7">
         <f t="shared" si="2"/>
         <v>443</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G27" s="28">
         <v>1999.0</v>
       </c>
       <c r="H27" s="35" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I27" s="28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K27" s="63">
         <v>44500.0</v>
@@ -3053,51 +3084,52 @@
       <c r="N27" s="32"/>
       <c r="O27" s="60"/>
       <c r="P27" s="37"/>
-      <c r="R27" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S27" s="33"/>
+      <c r="Q27" s="37"/>
+      <c r="S27" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="T27" s="33"/>
-      <c r="U27" s="34"/>
-      <c r="V27" s="33"/>
+      <c r="U27" s="33"/>
+      <c r="V27" s="34"/>
       <c r="W27" s="33"/>
       <c r="X27" s="33"/>
       <c r="Y27" s="33"/>
       <c r="Z27" s="33"/>
       <c r="AA27" s="33"/>
-      <c r="AB27" s="34"/>
+      <c r="AB27" s="33"/>
+      <c r="AC27" s="34"/>
     </row>
     <row r="28" ht="18.0" customHeight="1">
       <c r="A28" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B28" s="7">
         <f t="shared" si="2"/>
         <v>445</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G28" s="28">
         <v>1967.0</v>
       </c>
       <c r="H28" s="65" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I28" s="28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K28" s="63">
         <v>44504.0</v>
@@ -3109,50 +3141,51 @@
       <c r="N28" s="39"/>
       <c r="O28" s="43"/>
       <c r="P28" s="37"/>
-      <c r="R28" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S28" s="33"/>
+      <c r="Q28" s="37"/>
+      <c r="S28" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T28" s="33"/>
-      <c r="V28" s="33"/>
+      <c r="U28" s="33"/>
       <c r="W28" s="33"/>
       <c r="X28" s="33"/>
       <c r="Y28" s="33"/>
       <c r="Z28" s="33"/>
       <c r="AA28" s="33"/>
-      <c r="AB28" s="34"/>
+      <c r="AB28" s="33"/>
+      <c r="AC28" s="34"/>
     </row>
     <row r="29">
       <c r="A29" s="25" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B29" s="7">
         <f t="shared" si="2"/>
         <v>459</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G29" s="28">
         <v>1969.0</v>
       </c>
       <c r="H29" s="47" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I29" s="28" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K29" s="63">
         <v>44504.0</v>
@@ -3164,51 +3197,52 @@
       <c r="N29" s="39"/>
       <c r="O29" s="43"/>
       <c r="P29" s="32"/>
-      <c r="R29" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="S29" s="33"/>
+      <c r="Q29" s="32"/>
+      <c r="S29" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="T29" s="33"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="33"/>
+      <c r="U29" s="33"/>
+      <c r="V29" s="34"/>
       <c r="W29" s="33"/>
       <c r="X29" s="33"/>
       <c r="Y29" s="33"/>
       <c r="Z29" s="33"/>
       <c r="AA29" s="33"/>
-      <c r="AB29" s="34"/>
+      <c r="AB29" s="33"/>
+      <c r="AC29" s="34"/>
     </row>
     <row r="30">
       <c r="A30" s="25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B30" s="7">
         <f t="shared" si="2"/>
         <v>451</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G30" s="28">
         <v>2020.0</v>
       </c>
       <c r="H30" s="66" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I30" s="28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K30" s="63">
         <v>44505.0</v>
@@ -3224,51 +3258,52 @@
       </c>
       <c r="O30" s="40"/>
       <c r="P30" s="32"/>
-      <c r="R30" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="S30" s="33"/>
+      <c r="Q30" s="32"/>
+      <c r="S30" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="T30" s="33"/>
-      <c r="U30" s="34"/>
-      <c r="V30" s="33"/>
+      <c r="U30" s="33"/>
+      <c r="V30" s="34"/>
       <c r="W30" s="33"/>
       <c r="X30" s="33"/>
       <c r="Y30" s="33"/>
       <c r="Z30" s="33"/>
       <c r="AA30" s="33"/>
-      <c r="AB30" s="34"/>
+      <c r="AB30" s="33"/>
+      <c r="AC30" s="34"/>
     </row>
     <row r="31">
       <c r="A31" s="25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B31" s="7">
         <f t="shared" si="2"/>
         <v>454</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G31" s="28">
         <v>1984.0</v>
       </c>
       <c r="H31" s="35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I31" s="28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J31" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K31" s="48">
         <v>44506.0</v>
@@ -3280,51 +3315,52 @@
       <c r="N31" s="32"/>
       <c r="O31" s="32"/>
       <c r="P31" s="32"/>
-      <c r="R31" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S31" s="33"/>
+      <c r="Q31" s="32"/>
+      <c r="S31" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="T31" s="33"/>
-      <c r="U31" s="34"/>
-      <c r="V31" s="33"/>
+      <c r="U31" s="33"/>
+      <c r="V31" s="34"/>
       <c r="W31" s="33"/>
       <c r="X31" s="33"/>
       <c r="Y31" s="33"/>
       <c r="Z31" s="33"/>
       <c r="AA31" s="33"/>
-      <c r="AB31" s="34"/>
+      <c r="AB31" s="33"/>
+      <c r="AC31" s="34"/>
     </row>
     <row r="32">
       <c r="A32" s="25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B32" s="7">
         <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G32" s="28">
         <v>1971.0</v>
       </c>
       <c r="H32" s="62" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I32" s="28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J32" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K32" s="63">
         <v>44511.0</v>
@@ -3336,51 +3372,52 @@
       <c r="N32" s="32"/>
       <c r="O32" s="32"/>
       <c r="P32" s="32"/>
-      <c r="R32" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S32" s="33"/>
+      <c r="Q32" s="32"/>
+      <c r="S32" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T32" s="33"/>
-      <c r="U32" s="34"/>
-      <c r="V32" s="33"/>
+      <c r="U32" s="33"/>
+      <c r="V32" s="34"/>
       <c r="W32" s="33"/>
       <c r="X32" s="33"/>
       <c r="Y32" s="33"/>
       <c r="Z32" s="33"/>
       <c r="AA32" s="33"/>
-      <c r="AB32" s="34"/>
+      <c r="AB32" s="33"/>
+      <c r="AC32" s="34"/>
     </row>
     <row r="33">
       <c r="A33" s="54" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B33" s="7">
         <f t="shared" si="2"/>
         <v>443</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F33" s="54" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G33" s="55">
         <v>1974.0</v>
       </c>
       <c r="H33" s="52" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I33" s="55" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J33" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K33" s="63">
         <v>44511.0</v>
@@ -3392,51 +3429,52 @@
       <c r="N33" s="32"/>
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
-      <c r="R33" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="S33" s="33"/>
+      <c r="Q33" s="32"/>
+      <c r="S33" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="T33" s="33"/>
-      <c r="U33" s="34"/>
-      <c r="V33" s="33"/>
+      <c r="U33" s="33"/>
+      <c r="V33" s="34"/>
       <c r="W33" s="33"/>
       <c r="X33" s="33"/>
       <c r="Y33" s="33"/>
       <c r="Z33" s="33"/>
       <c r="AA33" s="33"/>
-      <c r="AB33" s="34"/>
+      <c r="AB33" s="33"/>
+      <c r="AC33" s="34"/>
     </row>
     <row r="34">
       <c r="A34" s="25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B34" s="7">
         <f t="shared" si="2"/>
         <v>442</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G34" s="28">
         <v>2021.0</v>
       </c>
       <c r="H34" s="35" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I34" s="28" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K34" s="63">
         <v>44512.0</v>
@@ -3452,50 +3490,51 @@
       </c>
       <c r="O34" s="32"/>
       <c r="P34" s="32"/>
-      <c r="R34" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="S34" s="33"/>
+      <c r="Q34" s="32"/>
+      <c r="S34" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="T34" s="33"/>
-      <c r="V34" s="33"/>
+      <c r="U34" s="33"/>
       <c r="W34" s="33"/>
       <c r="X34" s="33"/>
       <c r="Y34" s="33"/>
       <c r="Z34" s="33"/>
       <c r="AA34" s="33"/>
-      <c r="AB34" s="34"/>
+      <c r="AB34" s="33"/>
+      <c r="AC34" s="34"/>
     </row>
     <row r="35">
       <c r="A35" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B35" s="7">
         <f t="shared" si="2"/>
         <v>452</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G35" s="28">
         <v>1951.0</v>
       </c>
       <c r="H35" s="35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I35" s="28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J35" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K35" s="63">
         <v>44513.0</v>
@@ -3507,51 +3546,52 @@
       <c r="N35" s="32"/>
       <c r="O35" s="32"/>
       <c r="P35" s="32"/>
-      <c r="R35" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S35" s="33"/>
+      <c r="Q35" s="32"/>
+      <c r="S35" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="T35" s="33"/>
-      <c r="U35" s="34"/>
-      <c r="V35" s="33"/>
+      <c r="U35" s="33"/>
+      <c r="V35" s="34"/>
       <c r="W35" s="33"/>
       <c r="X35" s="33"/>
       <c r="Y35" s="33"/>
       <c r="Z35" s="33"/>
       <c r="AA35" s="33"/>
-      <c r="AB35" s="34"/>
+      <c r="AB35" s="33"/>
+      <c r="AC35" s="34"/>
     </row>
     <row r="36">
       <c r="A36" s="25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B36" s="7">
         <f t="shared" si="2"/>
         <v>447</v>
       </c>
       <c r="C36" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="25" t="s">
-        <v>38</v>
-      </c>
       <c r="E36" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G36" s="28">
         <v>1966.0</v>
       </c>
       <c r="H36" s="51" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I36" s="28" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J36" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K36" s="63">
         <v>44518.0</v>
@@ -3563,52 +3603,53 @@
       <c r="N36" s="37"/>
       <c r="O36" s="60"/>
       <c r="P36" s="37"/>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S36" s="33"/>
+      <c r="Q36" s="37"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T36" s="33"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="33"/>
+      <c r="U36" s="33"/>
+      <c r="V36" s="34"/>
       <c r="W36" s="33"/>
       <c r="X36" s="33"/>
       <c r="Y36" s="33"/>
       <c r="Z36" s="33"/>
       <c r="AA36" s="33"/>
-      <c r="AB36" s="34"/>
+      <c r="AB36" s="33"/>
+      <c r="AC36" s="34"/>
     </row>
     <row r="37">
       <c r="A37" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B37" s="7">
         <f t="shared" si="2"/>
         <v>458</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G37" s="28">
         <v>1956.0</v>
       </c>
       <c r="H37" s="47" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I37" s="28" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J37" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K37" s="63">
         <v>44518.0</v>
@@ -3620,51 +3661,52 @@
       <c r="N37" s="39"/>
       <c r="O37" s="43"/>
       <c r="P37" s="37"/>
-      <c r="Q37" s="27"/>
-      <c r="R37" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="S37" s="33"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="27"/>
+      <c r="S37" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="T37" s="33"/>
-      <c r="U37" s="34"/>
-      <c r="V37" s="33"/>
+      <c r="U37" s="33"/>
+      <c r="V37" s="34"/>
       <c r="W37" s="33"/>
-      <c r="X37" s="32"/>
+      <c r="X37" s="33"/>
       <c r="Y37" s="32"/>
-      <c r="Z37" s="33"/>
+      <c r="Z37" s="32"/>
       <c r="AA37" s="33"/>
+      <c r="AB37" s="33"/>
     </row>
     <row r="38">
       <c r="A38" s="25" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B38" s="7">
         <f t="shared" si="2"/>
         <v>443</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G38" s="28">
         <v>2020.0</v>
       </c>
       <c r="H38" s="35" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I38" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J38" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K38" s="63">
         <v>44519.0</v>
@@ -3680,50 +3722,51 @@
       </c>
       <c r="O38" s="43"/>
       <c r="P38" s="32"/>
-      <c r="R38" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="S38" s="33"/>
+      <c r="Q38" s="32"/>
+      <c r="S38" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="T38" s="33"/>
-      <c r="U38" s="34"/>
-      <c r="V38" s="32"/>
+      <c r="U38" s="33"/>
+      <c r="V38" s="34"/>
       <c r="W38" s="32"/>
       <c r="X38" s="32"/>
       <c r="Y38" s="32"/>
       <c r="Z38" s="32"/>
       <c r="AA38" s="32"/>
+      <c r="AB38" s="32"/>
     </row>
     <row r="39">
       <c r="A39" s="25" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B39" s="7">
         <f t="shared" si="2"/>
         <v>460</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G39" s="28">
         <v>1998.0</v>
       </c>
       <c r="H39" s="62" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I39" s="28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J39" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K39" s="48">
         <v>44520.0</v>
@@ -3735,51 +3778,52 @@
       <c r="N39" s="32"/>
       <c r="O39" s="32"/>
       <c r="P39" s="32"/>
-      <c r="R39" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S39" s="33"/>
+      <c r="Q39" s="32"/>
+      <c r="S39" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="T39" s="33"/>
-      <c r="U39" s="34"/>
-      <c r="V39" s="33"/>
+      <c r="U39" s="33"/>
+      <c r="V39" s="34"/>
       <c r="W39" s="33"/>
       <c r="X39" s="33"/>
       <c r="Y39" s="33"/>
       <c r="Z39" s="33"/>
       <c r="AA39" s="33"/>
-      <c r="AB39" s="34"/>
+      <c r="AB39" s="33"/>
+      <c r="AC39" s="34"/>
     </row>
     <row r="40">
       <c r="A40" s="25" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B40" s="7">
         <f t="shared" si="2"/>
         <v>458</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G40" s="25">
         <v>1954.0</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I40" s="25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J40" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K40" s="68">
         <v>44532.0</v>
@@ -3791,49 +3835,50 @@
       <c r="N40" s="32"/>
       <c r="O40" s="32"/>
       <c r="P40" s="32"/>
-      <c r="R40" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="S40" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="T40" s="32"/>
-      <c r="V40" s="32"/>
+      <c r="U40" s="32"/>
       <c r="W40" s="32"/>
       <c r="X40" s="32"/>
       <c r="Y40" s="32"/>
       <c r="Z40" s="32"/>
       <c r="AA40" s="32"/>
+      <c r="AB40" s="32"/>
     </row>
     <row r="41">
       <c r="A41" s="25" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B41" s="7">
         <f t="shared" si="2"/>
         <v>458</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G41" s="28">
         <v>2006.0</v>
       </c>
       <c r="H41" s="52" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I41" s="28" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J41" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K41" s="68">
         <v>44532.0</v>
@@ -3845,51 +3890,52 @@
       <c r="N41" s="32"/>
       <c r="O41" s="32"/>
       <c r="P41" s="32"/>
-      <c r="R41" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="S41" s="33"/>
+      <c r="Q41" s="32"/>
+      <c r="S41" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="T41" s="33"/>
-      <c r="U41" s="34"/>
-      <c r="V41" s="33"/>
+      <c r="U41" s="33"/>
+      <c r="V41" s="34"/>
       <c r="W41" s="33"/>
       <c r="X41" s="33"/>
       <c r="Y41" s="33"/>
       <c r="Z41" s="33"/>
       <c r="AA41" s="33"/>
-      <c r="AB41" s="34"/>
+      <c r="AB41" s="33"/>
+      <c r="AC41" s="34"/>
     </row>
     <row r="42">
       <c r="A42" s="25" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B42" s="7">
         <f t="shared" si="2"/>
         <v>458</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F42" s="54" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G42" s="55">
         <v>2021.0</v>
       </c>
       <c r="H42" s="35" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I42" s="28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J42" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K42" s="63">
         <v>44533.0</v>
@@ -3905,51 +3951,52 @@
       </c>
       <c r="O42" s="32"/>
       <c r="P42" s="32"/>
-      <c r="R42" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="S42" s="33"/>
+      <c r="Q42" s="32"/>
+      <c r="S42" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="T42" s="33"/>
-      <c r="U42" s="34"/>
-      <c r="V42" s="33"/>
+      <c r="U42" s="33"/>
+      <c r="V42" s="34"/>
       <c r="W42" s="33"/>
       <c r="X42" s="33"/>
       <c r="Y42" s="33"/>
       <c r="Z42" s="33"/>
       <c r="AA42" s="33"/>
-      <c r="AB42" s="34"/>
+      <c r="AB42" s="33"/>
+      <c r="AC42" s="34"/>
     </row>
     <row r="43">
       <c r="A43" s="25" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B43" s="7">
         <f t="shared" si="2"/>
         <v>454</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G43" s="28">
         <v>1998.0</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I43" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="J43" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K43" s="63">
         <v>44534.0</v>
@@ -3961,19 +4008,20 @@
       <c r="N43" s="32"/>
       <c r="O43" s="32"/>
       <c r="P43" s="32"/>
-      <c r="R43" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="S43" s="33"/>
+      <c r="Q43" s="32"/>
+      <c r="S43" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="T43" s="33"/>
-      <c r="U43" s="34"/>
-      <c r="V43" s="33"/>
+      <c r="U43" s="33"/>
+      <c r="V43" s="34"/>
       <c r="W43" s="33"/>
       <c r="X43" s="33"/>
       <c r="Y43" s="33"/>
       <c r="Z43" s="33"/>
       <c r="AA43" s="33"/>
-      <c r="AB43" s="34"/>
+      <c r="AB43" s="33"/>
+      <c r="AC43" s="34"/>
     </row>
     <row r="44">
       <c r="A44" s="25"/>
@@ -3991,16 +4039,17 @@
       <c r="N44" s="32"/>
       <c r="O44" s="60"/>
       <c r="P44" s="37"/>
-      <c r="S44" s="33"/>
+      <c r="Q44" s="37"/>
       <c r="T44" s="33"/>
-      <c r="U44" s="34"/>
-      <c r="V44" s="33"/>
+      <c r="U44" s="33"/>
+      <c r="V44" s="34"/>
       <c r="W44" s="33"/>
       <c r="X44" s="33"/>
       <c r="Y44" s="33"/>
       <c r="Z44" s="33"/>
       <c r="AA44" s="33"/>
-      <c r="AB44" s="34"/>
+      <c r="AB44" s="33"/>
+      <c r="AC44" s="34"/>
     </row>
     <row r="45">
       <c r="A45" s="25"/>
@@ -4017,17 +4066,18 @@
       <c r="N45" s="72"/>
       <c r="O45" s="43"/>
       <c r="P45" s="37"/>
-      <c r="Q45" s="49"/>
-      <c r="S45" s="33"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="49"/>
       <c r="T45" s="33"/>
-      <c r="U45" s="34"/>
-      <c r="V45" s="33"/>
+      <c r="U45" s="33"/>
+      <c r="V45" s="34"/>
       <c r="W45" s="33"/>
       <c r="X45" s="33"/>
       <c r="Y45" s="33"/>
       <c r="Z45" s="33"/>
       <c r="AA45" s="33"/>
-      <c r="AB45" s="34"/>
+      <c r="AB45" s="33"/>
+      <c r="AC45" s="34"/>
     </row>
     <row r="46">
       <c r="A46" s="25"/>
@@ -4044,17 +4094,18 @@
       <c r="N46" s="39"/>
       <c r="O46" s="43"/>
       <c r="P46" s="32"/>
-      <c r="Q46" s="49"/>
-      <c r="S46" s="33"/>
+      <c r="Q46" s="32"/>
+      <c r="R46" s="49"/>
       <c r="T46" s="33"/>
-      <c r="U46" s="34"/>
-      <c r="V46" s="33"/>
+      <c r="U46" s="33"/>
+      <c r="V46" s="34"/>
       <c r="W46" s="33"/>
       <c r="X46" s="33"/>
       <c r="Y46" s="33"/>
       <c r="Z46" s="33"/>
       <c r="AA46" s="33"/>
-      <c r="AB46" s="34"/>
+      <c r="AB46" s="33"/>
+      <c r="AC46" s="34"/>
     </row>
     <row r="47">
       <c r="A47" s="25"/>
@@ -4071,14 +4122,15 @@
       <c r="N47" s="32"/>
       <c r="O47" s="32"/>
       <c r="P47" s="32"/>
-      <c r="S47" s="32"/>
+      <c r="Q47" s="32"/>
       <c r="T47" s="32"/>
-      <c r="V47" s="32"/>
+      <c r="U47" s="32"/>
       <c r="W47" s="32"/>
       <c r="X47" s="32"/>
       <c r="Y47" s="32"/>
       <c r="Z47" s="32"/>
       <c r="AA47" s="32"/>
+      <c r="AB47" s="32"/>
     </row>
     <row r="48">
       <c r="A48" s="25"/>
@@ -4096,16 +4148,17 @@
       <c r="N48" s="32"/>
       <c r="O48" s="32"/>
       <c r="P48" s="32"/>
-      <c r="S48" s="33"/>
+      <c r="Q48" s="32"/>
       <c r="T48" s="33"/>
-      <c r="U48" s="34"/>
-      <c r="V48" s="33"/>
+      <c r="U48" s="33"/>
+      <c r="V48" s="34"/>
       <c r="W48" s="33"/>
       <c r="X48" s="33"/>
       <c r="Y48" s="33"/>
       <c r="Z48" s="33"/>
       <c r="AA48" s="33"/>
-      <c r="AB48" s="34"/>
+      <c r="AB48" s="33"/>
+      <c r="AC48" s="34"/>
     </row>
     <row r="49">
       <c r="A49" s="25"/>
@@ -4123,16 +4176,17 @@
       <c r="N49" s="32"/>
       <c r="O49" s="32"/>
       <c r="P49" s="32"/>
-      <c r="S49" s="33"/>
+      <c r="Q49" s="32"/>
       <c r="T49" s="33"/>
-      <c r="U49" s="34"/>
-      <c r="V49" s="33"/>
+      <c r="U49" s="33"/>
+      <c r="V49" s="34"/>
       <c r="W49" s="33"/>
       <c r="X49" s="33"/>
       <c r="Y49" s="33"/>
       <c r="Z49" s="33"/>
       <c r="AA49" s="33"/>
-      <c r="AB49" s="34"/>
+      <c r="AB49" s="33"/>
+      <c r="AC49" s="34"/>
     </row>
     <row r="50">
       <c r="A50" s="76"/>
@@ -4150,16 +4204,17 @@
       <c r="N50" s="32"/>
       <c r="O50" s="32"/>
       <c r="P50" s="32"/>
-      <c r="S50" s="33"/>
+      <c r="Q50" s="32"/>
       <c r="T50" s="33"/>
-      <c r="U50" s="34"/>
-      <c r="V50" s="33"/>
+      <c r="U50" s="33"/>
+      <c r="V50" s="34"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
       <c r="Y50" s="33"/>
       <c r="Z50" s="33"/>
       <c r="AA50" s="33"/>
-      <c r="AB50" s="34"/>
+      <c r="AB50" s="33"/>
+      <c r="AC50" s="34"/>
     </row>
     <row r="51">
       <c r="A51" s="25"/>
@@ -4177,16 +4232,17 @@
       <c r="N51" s="32"/>
       <c r="O51" s="32"/>
       <c r="P51" s="32"/>
-      <c r="S51" s="33"/>
+      <c r="Q51" s="32"/>
       <c r="T51" s="33"/>
-      <c r="U51" s="34"/>
-      <c r="V51" s="33"/>
+      <c r="U51" s="33"/>
+      <c r="V51" s="34"/>
       <c r="W51" s="33"/>
       <c r="X51" s="33"/>
       <c r="Y51" s="33"/>
       <c r="Z51" s="33"/>
       <c r="AA51" s="33"/>
-      <c r="AB51" s="34"/>
+      <c r="AB51" s="33"/>
+      <c r="AC51" s="34"/>
     </row>
     <row r="52">
       <c r="A52" s="25"/>
@@ -4204,17 +4260,18 @@
       <c r="N52" s="32"/>
       <c r="O52" s="60"/>
       <c r="P52" s="37"/>
-      <c r="Q52" s="49"/>
-      <c r="S52" s="33"/>
+      <c r="Q52" s="37"/>
+      <c r="R52" s="49"/>
       <c r="T52" s="33"/>
-      <c r="U52" s="34"/>
-      <c r="V52" s="33"/>
+      <c r="U52" s="33"/>
+      <c r="V52" s="34"/>
       <c r="W52" s="33"/>
       <c r="X52" s="33"/>
       <c r="Y52" s="33"/>
       <c r="Z52" s="33"/>
       <c r="AA52" s="33"/>
-      <c r="AB52" s="34"/>
+      <c r="AB52" s="33"/>
+      <c r="AC52" s="34"/>
     </row>
     <row r="53">
       <c r="A53" s="25"/>
@@ -4232,17 +4289,18 @@
       <c r="N53" s="32"/>
       <c r="O53" s="60"/>
       <c r="P53" s="37"/>
-      <c r="Q53" s="49"/>
-      <c r="S53" s="33"/>
+      <c r="Q53" s="37"/>
+      <c r="R53" s="49"/>
       <c r="T53" s="33"/>
-      <c r="U53" s="34"/>
-      <c r="V53" s="33"/>
+      <c r="U53" s="33"/>
+      <c r="V53" s="34"/>
       <c r="W53" s="33"/>
       <c r="X53" s="33"/>
       <c r="Y53" s="33"/>
       <c r="Z53" s="33"/>
       <c r="AA53" s="33"/>
-      <c r="AB53" s="34"/>
+      <c r="AB53" s="33"/>
+      <c r="AC53" s="34"/>
     </row>
     <row r="54">
       <c r="A54" s="25"/>
@@ -4259,16 +4317,17 @@
       <c r="N54" s="39"/>
       <c r="O54" s="43"/>
       <c r="P54" s="32"/>
-      <c r="S54" s="33"/>
+      <c r="Q54" s="32"/>
       <c r="T54" s="33"/>
-      <c r="U54" s="34"/>
-      <c r="V54" s="33"/>
+      <c r="U54" s="33"/>
+      <c r="V54" s="34"/>
       <c r="W54" s="33"/>
       <c r="X54" s="33"/>
       <c r="Y54" s="33"/>
       <c r="Z54" s="33"/>
       <c r="AA54" s="33"/>
-      <c r="AB54" s="34"/>
+      <c r="AB54" s="33"/>
+      <c r="AC54" s="34"/>
     </row>
     <row r="55">
       <c r="A55" s="25"/>
@@ -4286,16 +4345,17 @@
       <c r="N55" s="39"/>
       <c r="O55" s="43"/>
       <c r="P55" s="32"/>
-      <c r="S55" s="33"/>
+      <c r="Q55" s="32"/>
       <c r="T55" s="33"/>
-      <c r="U55" s="34"/>
-      <c r="V55" s="33"/>
+      <c r="U55" s="33"/>
+      <c r="V55" s="34"/>
       <c r="W55" s="33"/>
       <c r="X55" s="33"/>
       <c r="Y55" s="33"/>
       <c r="Z55" s="33"/>
       <c r="AA55" s="33"/>
-      <c r="AB55" s="34"/>
+      <c r="AB55" s="33"/>
+      <c r="AC55" s="34"/>
     </row>
     <row r="56">
       <c r="A56" s="25"/>
@@ -4313,16 +4373,17 @@
       <c r="N56" s="32"/>
       <c r="O56" s="32"/>
       <c r="P56" s="32"/>
-      <c r="S56" s="33"/>
+      <c r="Q56" s="32"/>
       <c r="T56" s="33"/>
-      <c r="U56" s="34"/>
-      <c r="V56" s="33"/>
+      <c r="U56" s="33"/>
+      <c r="V56" s="34"/>
       <c r="W56" s="33"/>
       <c r="X56" s="33"/>
       <c r="Y56" s="33"/>
       <c r="Z56" s="33"/>
       <c r="AA56" s="33"/>
-      <c r="AB56" s="34"/>
+      <c r="AB56" s="33"/>
+      <c r="AC56" s="34"/>
     </row>
     <row r="57">
       <c r="A57" s="25"/>
@@ -4340,16 +4401,17 @@
       <c r="N57" s="32"/>
       <c r="O57" s="32"/>
       <c r="P57" s="32"/>
-      <c r="S57" s="33"/>
+      <c r="Q57" s="32"/>
       <c r="T57" s="33"/>
-      <c r="U57" s="34"/>
-      <c r="V57" s="33"/>
+      <c r="U57" s="33"/>
+      <c r="V57" s="34"/>
       <c r="W57" s="33"/>
       <c r="X57" s="33"/>
       <c r="Y57" s="33"/>
       <c r="Z57" s="33"/>
       <c r="AA57" s="33"/>
-      <c r="AB57" s="34"/>
+      <c r="AB57" s="33"/>
+      <c r="AC57" s="34"/>
     </row>
     <row r="58">
       <c r="A58" s="25"/>
@@ -4367,16 +4429,17 @@
       <c r="N58" s="32"/>
       <c r="O58" s="32"/>
       <c r="P58" s="32"/>
-      <c r="S58" s="33"/>
+      <c r="Q58" s="32"/>
       <c r="T58" s="33"/>
-      <c r="U58" s="34"/>
-      <c r="V58" s="33"/>
+      <c r="U58" s="33"/>
+      <c r="V58" s="34"/>
       <c r="W58" s="33"/>
       <c r="X58" s="33"/>
       <c r="Y58" s="33"/>
       <c r="Z58" s="33"/>
       <c r="AA58" s="33"/>
-      <c r="AB58" s="34"/>
+      <c r="AB58" s="33"/>
+      <c r="AC58" s="34"/>
     </row>
     <row r="59">
       <c r="A59" s="25"/>
@@ -4394,17 +4457,18 @@
       <c r="N59" s="32"/>
       <c r="O59" s="32"/>
       <c r="P59" s="32"/>
-      <c r="Q59" s="49"/>
-      <c r="S59" s="33"/>
+      <c r="Q59" s="32"/>
+      <c r="R59" s="49"/>
       <c r="T59" s="33"/>
-      <c r="U59" s="34"/>
-      <c r="V59" s="33"/>
+      <c r="U59" s="33"/>
+      <c r="V59" s="34"/>
       <c r="W59" s="33"/>
       <c r="X59" s="33"/>
       <c r="Y59" s="33"/>
       <c r="Z59" s="33"/>
       <c r="AA59" s="33"/>
-      <c r="AB59" s="34"/>
+      <c r="AB59" s="33"/>
+      <c r="AC59" s="34"/>
     </row>
     <row r="60">
       <c r="A60" s="25"/>
@@ -4422,17 +4486,18 @@
       <c r="N60" s="37"/>
       <c r="O60" s="60"/>
       <c r="P60" s="37"/>
-      <c r="Q60" s="49"/>
-      <c r="S60" s="33"/>
+      <c r="Q60" s="37"/>
+      <c r="R60" s="49"/>
       <c r="T60" s="33"/>
-      <c r="U60" s="34"/>
-      <c r="V60" s="33"/>
+      <c r="U60" s="33"/>
+      <c r="V60" s="34"/>
       <c r="W60" s="33"/>
       <c r="X60" s="33"/>
       <c r="Y60" s="33"/>
       <c r="Z60" s="33"/>
       <c r="AA60" s="33"/>
-      <c r="AB60" s="34"/>
+      <c r="AB60" s="33"/>
+      <c r="AC60" s="34"/>
     </row>
     <row r="61">
       <c r="A61" s="25"/>
@@ -4450,16 +4515,17 @@
       <c r="N61" s="32"/>
       <c r="O61" s="60"/>
       <c r="P61" s="37"/>
-      <c r="S61" s="33"/>
+      <c r="Q61" s="37"/>
       <c r="T61" s="33"/>
-      <c r="U61" s="34"/>
-      <c r="V61" s="33"/>
+      <c r="U61" s="33"/>
+      <c r="V61" s="34"/>
       <c r="W61" s="33"/>
       <c r="X61" s="33"/>
       <c r="Y61" s="33"/>
       <c r="Z61" s="33"/>
       <c r="AA61" s="33"/>
-      <c r="AB61" s="34"/>
+      <c r="AB61" s="33"/>
+      <c r="AC61" s="34"/>
     </row>
     <row r="62">
       <c r="A62" s="25"/>
@@ -4477,17 +4543,18 @@
       <c r="N62" s="39"/>
       <c r="O62" s="43"/>
       <c r="P62" s="32"/>
-      <c r="Q62" s="49"/>
-      <c r="S62" s="33"/>
+      <c r="Q62" s="32"/>
+      <c r="R62" s="49"/>
       <c r="T62" s="33"/>
-      <c r="U62" s="34"/>
-      <c r="V62" s="33"/>
+      <c r="U62" s="33"/>
+      <c r="V62" s="34"/>
       <c r="W62" s="33"/>
       <c r="X62" s="33"/>
       <c r="Y62" s="33"/>
       <c r="Z62" s="33"/>
       <c r="AA62" s="33"/>
-      <c r="AB62" s="34"/>
+      <c r="AB62" s="33"/>
+      <c r="AC62" s="34"/>
     </row>
     <row r="63">
       <c r="A63" s="25"/>
@@ -4504,16 +4571,17 @@
       <c r="N63" s="39"/>
       <c r="O63" s="43"/>
       <c r="P63" s="32"/>
-      <c r="S63" s="33"/>
+      <c r="Q63" s="32"/>
       <c r="T63" s="33"/>
-      <c r="U63" s="34"/>
-      <c r="V63" s="33"/>
+      <c r="U63" s="33"/>
+      <c r="V63" s="34"/>
       <c r="W63" s="33"/>
       <c r="X63" s="33"/>
       <c r="Y63" s="33"/>
       <c r="Z63" s="33"/>
       <c r="AA63" s="33"/>
-      <c r="AB63" s="34"/>
+      <c r="AB63" s="33"/>
+      <c r="AC63" s="34"/>
     </row>
     <row r="64">
       <c r="A64" s="25"/>
@@ -4530,16 +4598,17 @@
       <c r="N64" s="32"/>
       <c r="O64" s="32"/>
       <c r="P64" s="32"/>
-      <c r="S64" s="33"/>
+      <c r="Q64" s="32"/>
       <c r="T64" s="33"/>
-      <c r="U64" s="34"/>
-      <c r="V64" s="33"/>
+      <c r="U64" s="33"/>
+      <c r="V64" s="34"/>
       <c r="W64" s="33"/>
       <c r="X64" s="33"/>
       <c r="Y64" s="33"/>
       <c r="Z64" s="33"/>
       <c r="AA64" s="33"/>
-      <c r="AB64" s="34"/>
+      <c r="AB64" s="33"/>
+      <c r="AC64" s="34"/>
     </row>
     <row r="65">
       <c r="A65" s="25"/>
@@ -4557,16 +4626,17 @@
       <c r="N65" s="32"/>
       <c r="O65" s="32"/>
       <c r="P65" s="32"/>
-      <c r="S65" s="33"/>
+      <c r="Q65" s="32"/>
       <c r="T65" s="33"/>
-      <c r="U65" s="34"/>
-      <c r="V65" s="33"/>
+      <c r="U65" s="33"/>
+      <c r="V65" s="34"/>
       <c r="W65" s="33"/>
       <c r="X65" s="33"/>
       <c r="Y65" s="33"/>
       <c r="Z65" s="33"/>
       <c r="AA65" s="33"/>
-      <c r="AB65" s="34"/>
+      <c r="AB65" s="33"/>
+      <c r="AC65" s="34"/>
     </row>
     <row r="66">
       <c r="A66" s="25"/>
@@ -4584,16 +4654,17 @@
       <c r="N66" s="32"/>
       <c r="O66" s="32"/>
       <c r="P66" s="32"/>
-      <c r="S66" s="33"/>
+      <c r="Q66" s="32"/>
       <c r="T66" s="33"/>
-      <c r="U66" s="34"/>
-      <c r="V66" s="33"/>
+      <c r="U66" s="33"/>
+      <c r="V66" s="34"/>
       <c r="W66" s="33"/>
       <c r="X66" s="33"/>
       <c r="Y66" s="33"/>
       <c r="Z66" s="33"/>
       <c r="AA66" s="33"/>
-      <c r="AB66" s="34"/>
+      <c r="AB66" s="33"/>
+      <c r="AC66" s="34"/>
     </row>
     <row r="67">
       <c r="A67" s="25"/>
@@ -4611,16 +4682,17 @@
       <c r="N67" s="32"/>
       <c r="O67" s="32"/>
       <c r="P67" s="32"/>
-      <c r="S67" s="84"/>
+      <c r="Q67" s="32"/>
       <c r="T67" s="84"/>
-      <c r="U67" s="34"/>
-      <c r="V67" s="33"/>
+      <c r="U67" s="84"/>
+      <c r="V67" s="34"/>
       <c r="W67" s="33"/>
       <c r="X67" s="33"/>
       <c r="Y67" s="33"/>
       <c r="Z67" s="33"/>
       <c r="AA67" s="33"/>
-      <c r="AB67" s="34"/>
+      <c r="AB67" s="33"/>
+      <c r="AC67" s="34"/>
     </row>
     <row r="68">
       <c r="A68" s="25"/>
@@ -4638,16 +4710,17 @@
       <c r="N68" s="32"/>
       <c r="O68" s="32"/>
       <c r="P68" s="32"/>
-      <c r="S68" s="33"/>
+      <c r="Q68" s="32"/>
       <c r="T68" s="33"/>
-      <c r="U68" s="34"/>
-      <c r="V68" s="33"/>
+      <c r="U68" s="33"/>
+      <c r="V68" s="34"/>
       <c r="W68" s="33"/>
       <c r="X68" s="33"/>
       <c r="Y68" s="33"/>
       <c r="Z68" s="33"/>
       <c r="AA68" s="33"/>
-      <c r="AB68" s="34"/>
+      <c r="AB68" s="33"/>
+      <c r="AC68" s="34"/>
     </row>
     <row r="69">
       <c r="A69" s="25"/>
@@ -4665,17 +4738,18 @@
       <c r="N69" s="32"/>
       <c r="O69" s="60"/>
       <c r="P69" s="37"/>
-      <c r="Q69" s="49"/>
-      <c r="S69" s="33"/>
+      <c r="Q69" s="37"/>
+      <c r="R69" s="49"/>
       <c r="T69" s="33"/>
-      <c r="U69" s="34"/>
-      <c r="V69" s="33"/>
+      <c r="U69" s="33"/>
+      <c r="V69" s="34"/>
       <c r="W69" s="33"/>
       <c r="X69" s="33"/>
       <c r="Y69" s="33"/>
       <c r="Z69" s="33"/>
       <c r="AA69" s="33"/>
-      <c r="AB69" s="34"/>
+      <c r="AB69" s="33"/>
+      <c r="AC69" s="34"/>
     </row>
     <row r="70">
       <c r="A70" s="25"/>
@@ -4693,16 +4767,17 @@
       <c r="N70" s="32"/>
       <c r="O70" s="60"/>
       <c r="P70" s="37"/>
-      <c r="S70" s="33"/>
+      <c r="Q70" s="37"/>
       <c r="T70" s="33"/>
-      <c r="U70" s="34"/>
-      <c r="V70" s="33"/>
+      <c r="U70" s="33"/>
+      <c r="V70" s="34"/>
       <c r="W70" s="33"/>
       <c r="X70" s="33"/>
       <c r="Y70" s="33"/>
       <c r="Z70" s="33"/>
       <c r="AA70" s="33"/>
-      <c r="AB70" s="34"/>
+      <c r="AB70" s="33"/>
+      <c r="AC70" s="34"/>
     </row>
     <row r="71">
       <c r="A71" s="25"/>
@@ -4719,16 +4794,17 @@
       <c r="N71" s="39"/>
       <c r="O71" s="43"/>
       <c r="P71" s="32"/>
-      <c r="S71" s="33"/>
+      <c r="Q71" s="32"/>
       <c r="T71" s="33"/>
-      <c r="U71" s="34"/>
-      <c r="V71" s="33"/>
+      <c r="U71" s="33"/>
+      <c r="V71" s="34"/>
       <c r="W71" s="33"/>
       <c r="X71" s="33"/>
       <c r="Y71" s="33"/>
       <c r="Z71" s="33"/>
       <c r="AA71" s="33"/>
-      <c r="AB71" s="34"/>
+      <c r="AB71" s="33"/>
+      <c r="AC71" s="34"/>
     </row>
     <row r="72">
       <c r="A72" s="25"/>
@@ -4745,16 +4821,17 @@
       <c r="N72" s="32"/>
       <c r="O72" s="32"/>
       <c r="P72" s="32"/>
-      <c r="S72" s="33"/>
+      <c r="Q72" s="32"/>
       <c r="T72" s="33"/>
-      <c r="U72" s="34"/>
-      <c r="V72" s="33"/>
+      <c r="U72" s="33"/>
+      <c r="V72" s="34"/>
       <c r="W72" s="33"/>
       <c r="X72" s="33"/>
       <c r="Y72" s="33"/>
       <c r="Z72" s="33"/>
       <c r="AA72" s="33"/>
-      <c r="AB72" s="34"/>
+      <c r="AB72" s="33"/>
+      <c r="AC72" s="34"/>
     </row>
     <row r="73">
       <c r="A73" s="25"/>
@@ -4771,15 +4848,16 @@
       <c r="N73" s="32"/>
       <c r="O73" s="32"/>
       <c r="P73" s="32"/>
-      <c r="S73" s="33"/>
+      <c r="Q73" s="32"/>
       <c r="T73" s="33"/>
-      <c r="U73" s="34"/>
-      <c r="V73" s="33"/>
+      <c r="U73" s="33"/>
+      <c r="V73" s="34"/>
       <c r="W73" s="33"/>
       <c r="X73" s="33"/>
       <c r="Y73" s="33"/>
       <c r="Z73" s="33"/>
       <c r="AA73" s="33"/>
+      <c r="AB73" s="33"/>
     </row>
     <row r="74">
       <c r="A74" s="25"/>
@@ -4797,16 +4875,17 @@
       <c r="N74" s="32"/>
       <c r="O74" s="32"/>
       <c r="P74" s="32"/>
-      <c r="S74" s="33"/>
+      <c r="Q74" s="32"/>
       <c r="T74" s="33"/>
-      <c r="U74" s="34"/>
-      <c r="V74" s="33"/>
+      <c r="U74" s="33"/>
+      <c r="V74" s="34"/>
       <c r="W74" s="33"/>
       <c r="X74" s="33"/>
       <c r="Y74" s="33"/>
       <c r="Z74" s="33"/>
       <c r="AA74" s="33"/>
-      <c r="AB74" s="34"/>
+      <c r="AB74" s="33"/>
+      <c r="AC74" s="34"/>
     </row>
     <row r="75">
       <c r="A75" s="25"/>
@@ -4824,16 +4903,17 @@
       <c r="N75" s="32"/>
       <c r="O75" s="32"/>
       <c r="P75" s="32"/>
-      <c r="S75" s="33"/>
+      <c r="Q75" s="32"/>
       <c r="T75" s="33"/>
-      <c r="U75" s="34"/>
-      <c r="V75" s="33"/>
+      <c r="U75" s="33"/>
+      <c r="V75" s="34"/>
       <c r="W75" s="33"/>
       <c r="X75" s="33"/>
       <c r="Y75" s="33"/>
       <c r="Z75" s="33"/>
       <c r="AA75" s="33"/>
-      <c r="AB75" s="34"/>
+      <c r="AB75" s="33"/>
+      <c r="AC75" s="34"/>
     </row>
     <row r="76">
       <c r="A76" s="88"/>
@@ -4852,16 +4932,17 @@
       <c r="N76" s="32"/>
       <c r="O76" s="32"/>
       <c r="P76" s="32"/>
-      <c r="S76" s="33"/>
+      <c r="Q76" s="32"/>
       <c r="T76" s="33"/>
-      <c r="U76" s="34"/>
-      <c r="V76" s="33"/>
+      <c r="U76" s="33"/>
+      <c r="V76" s="34"/>
       <c r="W76" s="33"/>
       <c r="X76" s="33"/>
       <c r="Y76" s="33"/>
       <c r="Z76" s="33"/>
       <c r="AA76" s="33"/>
-      <c r="AB76" s="34"/>
+      <c r="AB76" s="33"/>
+      <c r="AC76" s="34"/>
     </row>
     <row r="77">
       <c r="A77" s="25"/>
@@ -4879,16 +4960,17 @@
       <c r="N77" s="32"/>
       <c r="O77" s="60"/>
       <c r="P77" s="37"/>
-      <c r="S77" s="33"/>
+      <c r="Q77" s="37"/>
       <c r="T77" s="33"/>
-      <c r="U77" s="34"/>
-      <c r="V77" s="33"/>
+      <c r="U77" s="33"/>
+      <c r="V77" s="34"/>
       <c r="W77" s="33"/>
       <c r="X77" s="33"/>
       <c r="Y77" s="33"/>
       <c r="Z77" s="33"/>
       <c r="AA77" s="33"/>
-      <c r="AB77" s="34"/>
+      <c r="AB77" s="33"/>
+      <c r="AC77" s="34"/>
     </row>
     <row r="78">
       <c r="A78" s="25"/>
@@ -4906,16 +4988,17 @@
       <c r="N78" s="32"/>
       <c r="O78" s="60"/>
       <c r="P78" s="37"/>
-      <c r="S78" s="33"/>
+      <c r="Q78" s="37"/>
       <c r="T78" s="33"/>
-      <c r="U78" s="34"/>
-      <c r="V78" s="33"/>
+      <c r="U78" s="33"/>
+      <c r="V78" s="34"/>
       <c r="W78" s="33"/>
       <c r="X78" s="33"/>
       <c r="Y78" s="33"/>
       <c r="Z78" s="33"/>
       <c r="AA78" s="33"/>
-      <c r="AB78" s="34"/>
+      <c r="AB78" s="33"/>
+      <c r="AC78" s="34"/>
     </row>
     <row r="79">
       <c r="A79" s="25"/>
@@ -4932,16 +5015,17 @@
       <c r="M79" s="32"/>
       <c r="N79" s="32"/>
       <c r="P79" s="32"/>
-      <c r="S79" s="33"/>
+      <c r="Q79" s="32"/>
       <c r="T79" s="33"/>
-      <c r="U79" s="34"/>
-      <c r="V79" s="33"/>
+      <c r="U79" s="33"/>
+      <c r="V79" s="34"/>
       <c r="W79" s="33"/>
       <c r="X79" s="33"/>
       <c r="Y79" s="33"/>
       <c r="Z79" s="33"/>
       <c r="AA79" s="33"/>
-      <c r="AB79" s="34"/>
+      <c r="AB79" s="33"/>
+      <c r="AC79" s="34"/>
     </row>
     <row r="80">
       <c r="A80" s="25"/>
@@ -4958,16 +5042,17 @@
       <c r="M80" s="32"/>
       <c r="N80" s="32"/>
       <c r="P80" s="32"/>
-      <c r="S80" s="33"/>
+      <c r="Q80" s="32"/>
       <c r="T80" s="33"/>
-      <c r="U80" s="34"/>
-      <c r="V80" s="33"/>
+      <c r="U80" s="33"/>
+      <c r="V80" s="34"/>
       <c r="W80" s="33"/>
       <c r="X80" s="33"/>
       <c r="Y80" s="33"/>
       <c r="Z80" s="33"/>
       <c r="AA80" s="33"/>
-      <c r="AB80" s="34"/>
+      <c r="AB80" s="33"/>
+      <c r="AC80" s="34"/>
     </row>
     <row r="81">
       <c r="A81" s="25"/>
@@ -4985,16 +5070,17 @@
       <c r="N81" s="39"/>
       <c r="O81" s="43"/>
       <c r="P81" s="32"/>
-      <c r="S81" s="33"/>
+      <c r="Q81" s="32"/>
       <c r="T81" s="33"/>
-      <c r="U81" s="34"/>
-      <c r="V81" s="33"/>
+      <c r="U81" s="33"/>
+      <c r="V81" s="34"/>
       <c r="W81" s="33"/>
       <c r="X81" s="33"/>
       <c r="Y81" s="33"/>
       <c r="Z81" s="33"/>
       <c r="AA81" s="33"/>
-      <c r="AB81" s="34"/>
+      <c r="AB81" s="33"/>
+      <c r="AC81" s="34"/>
     </row>
     <row r="82">
       <c r="A82" s="54"/>
@@ -5012,16 +5098,17 @@
       <c r="N82" s="39"/>
       <c r="O82" s="43"/>
       <c r="P82" s="32"/>
-      <c r="S82" s="33"/>
+      <c r="Q82" s="32"/>
       <c r="T82" s="33"/>
-      <c r="U82" s="34"/>
-      <c r="V82" s="33"/>
+      <c r="U82" s="33"/>
+      <c r="V82" s="34"/>
       <c r="W82" s="33"/>
       <c r="X82" s="33"/>
       <c r="Y82" s="33"/>
       <c r="Z82" s="33"/>
       <c r="AA82" s="33"/>
-      <c r="AB82" s="34"/>
+      <c r="AB82" s="33"/>
+      <c r="AC82" s="34"/>
     </row>
     <row r="83">
       <c r="A83" s="25"/>
@@ -5038,16 +5125,17 @@
       <c r="N83" s="32"/>
       <c r="O83" s="32"/>
       <c r="P83" s="32"/>
-      <c r="S83" s="33"/>
+      <c r="Q83" s="32"/>
       <c r="T83" s="33"/>
-      <c r="U83" s="34"/>
-      <c r="V83" s="33"/>
+      <c r="U83" s="33"/>
+      <c r="V83" s="34"/>
       <c r="W83" s="33"/>
       <c r="X83" s="33"/>
       <c r="Y83" s="33"/>
       <c r="Z83" s="33"/>
       <c r="AA83" s="33"/>
-      <c r="AB83" s="34"/>
+      <c r="AB83" s="33"/>
+      <c r="AC83" s="34"/>
     </row>
     <row r="84">
       <c r="A84" s="25"/>
@@ -5066,16 +5154,17 @@
       <c r="N84" s="32"/>
       <c r="O84" s="32"/>
       <c r="P84" s="32"/>
-      <c r="S84" s="33"/>
+      <c r="Q84" s="32"/>
       <c r="T84" s="33"/>
-      <c r="U84" s="34"/>
-      <c r="V84" s="33"/>
+      <c r="U84" s="33"/>
+      <c r="V84" s="34"/>
       <c r="W84" s="33"/>
       <c r="X84" s="33"/>
       <c r="Y84" s="33"/>
       <c r="Z84" s="33"/>
       <c r="AA84" s="33"/>
-      <c r="AB84" s="34"/>
+      <c r="AB84" s="33"/>
+      <c r="AC84" s="34"/>
     </row>
     <row r="85">
       <c r="A85" s="25"/>
@@ -5094,16 +5183,17 @@
       <c r="N85" s="32"/>
       <c r="O85" s="32"/>
       <c r="P85" s="32"/>
-      <c r="S85" s="33"/>
+      <c r="Q85" s="32"/>
       <c r="T85" s="33"/>
-      <c r="U85" s="34"/>
-      <c r="V85" s="33"/>
+      <c r="U85" s="33"/>
+      <c r="V85" s="34"/>
       <c r="W85" s="33"/>
       <c r="X85" s="33"/>
       <c r="Y85" s="33"/>
       <c r="Z85" s="33"/>
       <c r="AA85" s="33"/>
-      <c r="AB85" s="34"/>
+      <c r="AB85" s="33"/>
+      <c r="AC85" s="34"/>
     </row>
     <row r="86">
       <c r="A86" s="25"/>
@@ -5122,17 +5212,18 @@
       <c r="N86" s="37"/>
       <c r="O86" s="60"/>
       <c r="P86" s="37"/>
-      <c r="Q86" s="49"/>
-      <c r="S86" s="33"/>
+      <c r="Q86" s="37"/>
+      <c r="R86" s="49"/>
       <c r="T86" s="33"/>
-      <c r="U86" s="34"/>
-      <c r="V86" s="33"/>
+      <c r="U86" s="33"/>
+      <c r="V86" s="34"/>
       <c r="W86" s="33"/>
       <c r="X86" s="33"/>
       <c r="Y86" s="33"/>
       <c r="Z86" s="33"/>
       <c r="AA86" s="33"/>
-      <c r="AB86" s="34"/>
+      <c r="AB86" s="33"/>
+      <c r="AC86" s="34"/>
     </row>
     <row r="87">
       <c r="A87" s="25"/>
@@ -5151,17 +5242,18 @@
       <c r="N87" s="32"/>
       <c r="O87" s="60"/>
       <c r="P87" s="37"/>
-      <c r="Q87" s="49"/>
-      <c r="S87" s="33"/>
+      <c r="Q87" s="37"/>
+      <c r="R87" s="49"/>
       <c r="T87" s="33"/>
-      <c r="U87" s="34"/>
-      <c r="V87" s="33"/>
+      <c r="U87" s="33"/>
+      <c r="V87" s="34"/>
       <c r="W87" s="33"/>
       <c r="X87" s="33"/>
       <c r="Y87" s="33"/>
       <c r="Z87" s="33"/>
       <c r="AA87" s="33"/>
-      <c r="AB87" s="34"/>
+      <c r="AB87" s="33"/>
+      <c r="AC87" s="34"/>
     </row>
     <row r="88">
       <c r="A88" s="25"/>
@@ -5179,16 +5271,17 @@
       <c r="M88" s="32"/>
       <c r="N88" s="32"/>
       <c r="P88" s="32"/>
-      <c r="S88" s="33"/>
+      <c r="Q88" s="32"/>
       <c r="T88" s="33"/>
-      <c r="U88" s="34"/>
-      <c r="V88" s="33"/>
+      <c r="U88" s="33"/>
+      <c r="V88" s="34"/>
       <c r="W88" s="33"/>
       <c r="X88" s="33"/>
       <c r="Y88" s="33"/>
       <c r="Z88" s="33"/>
       <c r="AA88" s="33"/>
-      <c r="AB88" s="34"/>
+      <c r="AB88" s="33"/>
+      <c r="AC88" s="34"/>
     </row>
     <row r="89">
       <c r="A89" s="93"/>
@@ -5206,16 +5299,17 @@
       <c r="M89" s="32"/>
       <c r="N89" s="32"/>
       <c r="P89" s="32"/>
-      <c r="S89" s="33"/>
+      <c r="Q89" s="32"/>
       <c r="T89" s="33"/>
-      <c r="U89" s="34"/>
-      <c r="V89" s="33"/>
+      <c r="U89" s="33"/>
+      <c r="V89" s="34"/>
       <c r="W89" s="33"/>
       <c r="X89" s="33"/>
       <c r="Y89" s="33"/>
       <c r="Z89" s="33"/>
       <c r="AA89" s="33"/>
-      <c r="AB89" s="34"/>
+      <c r="AB89" s="33"/>
+      <c r="AC89" s="34"/>
     </row>
     <row r="90">
       <c r="A90" s="93"/>
@@ -5233,16 +5327,17 @@
       <c r="M90" s="32"/>
       <c r="N90" s="32"/>
       <c r="P90" s="32"/>
-      <c r="S90" s="33"/>
+      <c r="Q90" s="32"/>
       <c r="T90" s="33"/>
-      <c r="U90" s="34"/>
-      <c r="V90" s="33"/>
+      <c r="U90" s="33"/>
+      <c r="V90" s="34"/>
       <c r="W90" s="33"/>
       <c r="X90" s="33"/>
       <c r="Y90" s="33"/>
       <c r="Z90" s="33"/>
       <c r="AA90" s="33"/>
-      <c r="AB90" s="34"/>
+      <c r="AB90" s="33"/>
+      <c r="AC90" s="34"/>
     </row>
     <row r="91">
       <c r="A91" s="50"/>
@@ -5260,16 +5355,17 @@
       <c r="M91" s="32"/>
       <c r="N91" s="32"/>
       <c r="P91" s="32"/>
-      <c r="S91" s="33"/>
+      <c r="Q91" s="32"/>
       <c r="T91" s="33"/>
-      <c r="U91" s="34"/>
-      <c r="V91" s="33"/>
+      <c r="U91" s="33"/>
+      <c r="V91" s="34"/>
       <c r="W91" s="33"/>
       <c r="X91" s="33"/>
       <c r="Y91" s="33"/>
       <c r="Z91" s="33"/>
       <c r="AA91" s="33"/>
-      <c r="AB91" s="34"/>
+      <c r="AB91" s="33"/>
+      <c r="AC91" s="34"/>
     </row>
     <row r="92">
       <c r="A92" s="50"/>
@@ -5287,16 +5383,17 @@
       <c r="M92" s="32"/>
       <c r="N92" s="32"/>
       <c r="P92" s="32"/>
-      <c r="S92" s="33"/>
+      <c r="Q92" s="32"/>
       <c r="T92" s="33"/>
-      <c r="U92" s="34"/>
-      <c r="V92" s="33"/>
+      <c r="U92" s="33"/>
+      <c r="V92" s="34"/>
       <c r="W92" s="33"/>
       <c r="X92" s="33"/>
       <c r="Y92" s="33"/>
       <c r="Z92" s="33"/>
       <c r="AA92" s="33"/>
-      <c r="AB92" s="34"/>
+      <c r="AB92" s="33"/>
+      <c r="AC92" s="34"/>
     </row>
     <row r="93">
       <c r="A93" s="50"/>
@@ -5314,16 +5411,17 @@
       <c r="M93" s="32"/>
       <c r="N93" s="32"/>
       <c r="P93" s="32"/>
-      <c r="S93" s="33"/>
+      <c r="Q93" s="32"/>
       <c r="T93" s="33"/>
-      <c r="U93" s="34"/>
-      <c r="V93" s="33"/>
+      <c r="U93" s="33"/>
+      <c r="V93" s="34"/>
       <c r="W93" s="33"/>
       <c r="X93" s="33"/>
       <c r="Y93" s="33"/>
       <c r="Z93" s="33"/>
       <c r="AA93" s="33"/>
-      <c r="AB93" s="34"/>
+      <c r="AB93" s="33"/>
+      <c r="AC93" s="34"/>
     </row>
     <row r="94">
       <c r="A94" s="50"/>
@@ -5341,16 +5439,17 @@
       <c r="M94" s="32"/>
       <c r="N94" s="32"/>
       <c r="P94" s="32"/>
-      <c r="S94" s="33"/>
+      <c r="Q94" s="32"/>
       <c r="T94" s="33"/>
-      <c r="U94" s="34"/>
-      <c r="V94" s="33"/>
+      <c r="U94" s="33"/>
+      <c r="V94" s="34"/>
       <c r="W94" s="33"/>
       <c r="X94" s="33"/>
       <c r="Y94" s="33"/>
       <c r="Z94" s="33"/>
       <c r="AA94" s="33"/>
-      <c r="AB94" s="34"/>
+      <c r="AB94" s="33"/>
+      <c r="AC94" s="34"/>
     </row>
     <row r="95">
       <c r="A95" s="50"/>
@@ -5368,16 +5467,17 @@
       <c r="M95" s="32"/>
       <c r="N95" s="32"/>
       <c r="P95" s="32"/>
-      <c r="S95" s="33"/>
+      <c r="Q95" s="32"/>
       <c r="T95" s="33"/>
-      <c r="U95" s="34"/>
-      <c r="V95" s="33"/>
+      <c r="U95" s="33"/>
+      <c r="V95" s="34"/>
       <c r="W95" s="33"/>
       <c r="X95" s="33"/>
       <c r="Y95" s="33"/>
       <c r="Z95" s="33"/>
       <c r="AA95" s="33"/>
-      <c r="AB95" s="34"/>
+      <c r="AB95" s="33"/>
+      <c r="AC95" s="34"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E54 F45">
@@ -5526,13 +5626,13 @@
   <sheetData>
     <row r="1" ht="33.75" customHeight="1">
       <c r="A1" s="101" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="101" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C1" s="101" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D1" s="102" t="s">
         <v>3</v>
@@ -5541,13 +5641,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="101" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G1" s="101" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H1" s="101" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I1" s="102"/>
       <c r="J1" s="102"/>
@@ -5563,29 +5663,29 @@
     </row>
     <row r="2" ht="65.25" customHeight="1">
       <c r="A2" s="104" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B2" s="105">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(F2="""","""",COUNTA(SPLIT(F2,"" "")))"),107.0)</f>
         <v>107</v>
       </c>
       <c r="C2" s="106" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="107" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2" s="106" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" s="108" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G2" s="109" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="110" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I2" s="109"/>
       <c r="J2" s="104"/>
@@ -5601,26 +5701,26 @@
     </row>
     <row r="3">
       <c r="A3" s="116" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B3" s="105">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(F3="""","""",COUNTA(SPLIT(F3,"" "")))"),41.0)</f>
         <v>41</v>
       </c>
       <c r="C3" s="117" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D3" s="118" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E3" s="119" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F3" s="120" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G3" s="121" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H3" s="122"/>
       <c r="I3" s="121"/>
@@ -5637,26 +5737,26 @@
     </row>
     <row r="4">
       <c r="A4" s="116" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B4" s="105">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(F4="""","""",COUNTA(SPLIT(F4,"" "")))"),211.0)</f>
         <v>211</v>
       </c>
       <c r="C4" s="119" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D4" s="123" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" s="119" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F4" s="132" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G4" s="121" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H4" s="119"/>
       <c r="I4" s="121"/>
@@ -5673,7 +5773,7 @@
     </row>
     <row r="5">
       <c r="A5" s="116" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B5" s="105" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(F5="""","""",COUNTA(SPLIT(F5,"" "")))"),"")</f>
@@ -5684,7 +5784,7 @@
       <c r="E5" s="119"/>
       <c r="F5" s="135"/>
       <c r="G5" s="121" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H5" s="120"/>
       <c r="I5" s="121"/>
@@ -5701,26 +5801,26 @@
     </row>
     <row r="6">
       <c r="A6" s="116" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B6" s="105">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(F6="""","""",COUNTA(SPLIT(F6,"" "")))"),171.0)</f>
         <v>171</v>
       </c>
       <c r="C6" s="119" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D6" s="123" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="119" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6" s="132" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G6" s="121" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H6" s="120"/>
       <c r="I6" s="121"/>
@@ -5737,7 +5837,7 @@
     </row>
     <row r="7">
       <c r="A7" s="139" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B7" s="105" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(F7="""","""",COUNTA(SPLIT(F7,"" "")))"),"")</f>
@@ -5748,7 +5848,7 @@
       <c r="E7" s="119"/>
       <c r="F7" s="132"/>
       <c r="G7" s="121" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H7" s="140"/>
       <c r="I7" s="121"/>

</xml_diff>